<commit_message>
update dl ngoc hoan
</commit_message>
<xml_diff>
--- a/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2023/Thang2/02.XuLyBH/XLBH2302_NgocHoan.xlsx
+++ b/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2023/Thang2/02.XuLyBH/XLBH2302_NgocHoan.xlsx
@@ -698,6 +698,30 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -713,32 +737,8 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1046,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X57"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1079,43 +1079,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="82"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="74"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
       <c r="W1" s="42"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="75" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="85" t="s">
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="77" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="85"/>
+      <c r="F2" s="77"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -1160,58 +1160,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="86" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="81" t="s">
+      <c r="A4" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81" t="s">
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="81"/>
-      <c r="L4" s="78" t="s">
+      <c r="K4" s="73"/>
+      <c r="L4" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="78" t="s">
+      <c r="M4" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="N4" s="78" t="s">
+      <c r="N4" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="78" t="s">
+      <c r="O4" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="76" t="s">
+      <c r="P4" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="78" t="s">
+      <c r="Q4" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="R4" s="78" t="s">
+      <c r="R4" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="S4" s="80" t="s">
+      <c r="S4" s="86" t="s">
         <v>52</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="81" t="s">
+      <c r="U4" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="V4" s="81" t="s">
+      <c r="V4" s="73" t="s">
         <v>51</v>
       </c>
       <c r="W4" s="43"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="86"/>
+      <c r="A5" s="78"/>
       <c r="B5" s="62" t="s">
         <v>1</v>
       </c>
@@ -1242,17 +1242,17 @@
       <c r="K5" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="79"/>
-      <c r="M5" s="79"/>
-      <c r="N5" s="79"/>
-      <c r="O5" s="79"/>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="79"/>
-      <c r="R5" s="79"/>
-      <c r="S5" s="80"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="80"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="80"/>
+      <c r="R5" s="80"/>
+      <c r="S5" s="86"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="81"/>
+      <c r="U5" s="73"/>
+      <c r="V5" s="73"/>
       <c r="W5" s="43"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1304,7 +1304,7 @@
       </c>
       <c r="S6" s="69"/>
       <c r="T6" s="63"/>
-      <c r="U6" s="73" t="s">
+      <c r="U6" s="81" t="s">
         <v>16</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -1365,7 +1365,7 @@
       </c>
       <c r="S7" s="3"/>
       <c r="T7" s="63"/>
-      <c r="U7" s="74"/>
+      <c r="U7" s="82"/>
       <c r="V7" s="3" t="s">
         <v>33</v>
       </c>
@@ -1394,7 +1394,7 @@
       <c r="R8" s="36"/>
       <c r="S8" s="3"/>
       <c r="T8" s="63"/>
-      <c r="U8" s="74"/>
+      <c r="U8" s="82"/>
       <c r="V8" s="3" t="s">
         <v>19</v>
       </c>
@@ -1423,7 +1423,7 @@
       <c r="R9" s="36"/>
       <c r="S9" s="3"/>
       <c r="T9" s="63"/>
-      <c r="U9" s="74"/>
+      <c r="U9" s="82"/>
       <c r="V9" s="3" t="s">
         <v>49</v>
       </c>
@@ -1452,7 +1452,7 @@
       <c r="R10" s="36"/>
       <c r="S10" s="3"/>
       <c r="T10" s="63"/>
-      <c r="U10" s="74"/>
+      <c r="U10" s="82"/>
       <c r="V10" s="3" t="s">
         <v>29</v>
       </c>
@@ -1481,7 +1481,7 @@
       <c r="R11" s="36"/>
       <c r="S11" s="3"/>
       <c r="T11" s="63"/>
-      <c r="U11" s="74"/>
+      <c r="U11" s="82"/>
       <c r="V11" s="3" t="s">
         <v>28</v>
       </c>
@@ -1510,7 +1510,7 @@
       <c r="R12" s="36"/>
       <c r="S12" s="3"/>
       <c r="T12" s="63"/>
-      <c r="U12" s="73" t="s">
+      <c r="U12" s="81" t="s">
         <v>17</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -1541,7 +1541,7 @@
       <c r="R13" s="36"/>
       <c r="S13" s="3"/>
       <c r="T13" s="63"/>
-      <c r="U13" s="74"/>
+      <c r="U13" s="82"/>
       <c r="V13" s="3" t="s">
         <v>35</v>
       </c>
@@ -1570,7 +1570,7 @@
       <c r="R14" s="36"/>
       <c r="S14" s="3"/>
       <c r="T14" s="63"/>
-      <c r="U14" s="74"/>
+      <c r="U14" s="82"/>
       <c r="V14" s="3" t="s">
         <v>34</v>
       </c>
@@ -1599,7 +1599,7 @@
       <c r="R15" s="36"/>
       <c r="S15" s="3"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="74"/>
+      <c r="U15" s="82"/>
       <c r="V15" s="3" t="s">
         <v>22</v>
       </c>
@@ -1628,7 +1628,7 @@
       <c r="R16" s="36"/>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="75"/>
+      <c r="U16" s="83"/>
       <c r="V16" s="3" t="s">
         <v>23</v>
       </c>
@@ -2856,6 +2856,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -2867,13 +2874,6 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2917,43 +2917,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="82"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="74"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
       <c r="W1" s="42"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="75" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="85" t="s">
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="77" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="85"/>
+      <c r="F2" s="77"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -2998,58 +2998,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="86" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="81" t="s">
+      <c r="A4" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81" t="s">
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="81"/>
-      <c r="L4" s="78" t="s">
+      <c r="K4" s="73"/>
+      <c r="L4" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="78" t="s">
+      <c r="M4" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="N4" s="78" t="s">
+      <c r="N4" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="78" t="s">
+      <c r="O4" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="76" t="s">
+      <c r="P4" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="78" t="s">
+      <c r="Q4" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="R4" s="78" t="s">
+      <c r="R4" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="S4" s="80" t="s">
+      <c r="S4" s="86" t="s">
         <v>52</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="81" t="s">
+      <c r="U4" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="V4" s="81" t="s">
+      <c r="V4" s="73" t="s">
         <v>51</v>
       </c>
       <c r="W4" s="43"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="86"/>
+      <c r="A5" s="78"/>
       <c r="B5" s="70" t="s">
         <v>1</v>
       </c>
@@ -3080,17 +3080,17 @@
       <c r="K5" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="79"/>
-      <c r="M5" s="79"/>
-      <c r="N5" s="79"/>
-      <c r="O5" s="79"/>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="79"/>
-      <c r="R5" s="79"/>
-      <c r="S5" s="80"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="80"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="80"/>
+      <c r="R5" s="80"/>
+      <c r="S5" s="86"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="81"/>
+      <c r="U5" s="73"/>
+      <c r="V5" s="73"/>
       <c r="W5" s="43"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3116,7 +3116,7 @@
       <c r="R6" s="61"/>
       <c r="S6" s="69"/>
       <c r="T6" s="63"/>
-      <c r="U6" s="73" t="s">
+      <c r="U6" s="81" t="s">
         <v>16</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -3147,7 +3147,7 @@
       <c r="R7" s="61"/>
       <c r="S7" s="3"/>
       <c r="T7" s="63"/>
-      <c r="U7" s="74"/>
+      <c r="U7" s="82"/>
       <c r="V7" s="3" t="s">
         <v>33</v>
       </c>
@@ -3176,7 +3176,7 @@
       <c r="R8" s="36"/>
       <c r="S8" s="3"/>
       <c r="T8" s="63"/>
-      <c r="U8" s="74"/>
+      <c r="U8" s="82"/>
       <c r="V8" s="3" t="s">
         <v>19</v>
       </c>
@@ -3205,7 +3205,7 @@
       <c r="R9" s="36"/>
       <c r="S9" s="3"/>
       <c r="T9" s="63"/>
-      <c r="U9" s="74"/>
+      <c r="U9" s="82"/>
       <c r="V9" s="3" t="s">
         <v>49</v>
       </c>
@@ -3234,7 +3234,7 @@
       <c r="R10" s="36"/>
       <c r="S10" s="3"/>
       <c r="T10" s="63"/>
-      <c r="U10" s="74"/>
+      <c r="U10" s="82"/>
       <c r="V10" s="3" t="s">
         <v>29</v>
       </c>
@@ -3263,7 +3263,7 @@
       <c r="R11" s="36"/>
       <c r="S11" s="3"/>
       <c r="T11" s="63"/>
-      <c r="U11" s="74"/>
+      <c r="U11" s="82"/>
       <c r="V11" s="3" t="s">
         <v>28</v>
       </c>
@@ -3292,7 +3292,7 @@
       <c r="R12" s="36"/>
       <c r="S12" s="3"/>
       <c r="T12" s="63"/>
-      <c r="U12" s="73" t="s">
+      <c r="U12" s="81" t="s">
         <v>17</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -3323,7 +3323,7 @@
       <c r="R13" s="36"/>
       <c r="S13" s="3"/>
       <c r="T13" s="63"/>
-      <c r="U13" s="74"/>
+      <c r="U13" s="82"/>
       <c r="V13" s="3" t="s">
         <v>35</v>
       </c>
@@ -3352,7 +3352,7 @@
       <c r="R14" s="36"/>
       <c r="S14" s="3"/>
       <c r="T14" s="63"/>
-      <c r="U14" s="74"/>
+      <c r="U14" s="82"/>
       <c r="V14" s="3" t="s">
         <v>34</v>
       </c>
@@ -3381,7 +3381,7 @@
       <c r="R15" s="36"/>
       <c r="S15" s="3"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="74"/>
+      <c r="U15" s="82"/>
       <c r="V15" s="3" t="s">
         <v>22</v>
       </c>
@@ -3410,7 +3410,7 @@
       <c r="R16" s="36"/>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="75"/>
+      <c r="U16" s="83"/>
       <c r="V16" s="3" t="s">
         <v>23</v>
       </c>
@@ -4638,13 +4638,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -4656,6 +4649,13 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>